<commit_message>
recursive update to sbol2 assembly untested
</commit_message>
<xml_diff>
--- a/scripts/SBOL_xlsx2.xlsx
+++ b/scripts/SBOL_xlsx2.xlsx
@@ -43,31 +43,31 @@
     <t>A4</t>
   </si>
   <si>
+    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/B0015/1</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/ComponentDefinition_dvk_backbone_core/1</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/J23100/1</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
     <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/B0032/1</t>
   </si>
   <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/ComponentDefinition_dvk_backbone_core/1</t>
-  </si>
-  <si>
-    <t>A6</t>
+    <t>B2</t>
   </si>
   <si>
     <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/E0040m_gfp/1</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/B0015/1</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/J23100/1</t>
   </si>
   <si>
     <t>B3</t>

</xml_diff>

<commit_message>
revert back to old
</commit_message>
<xml_diff>
--- a/scripts/SBOL_xlsx2.xlsx
+++ b/scripts/SBOL_xlsx2.xlsx
@@ -43,19 +43,19 @@
     <t>A4</t>
   </si>
   <si>
+    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/B0015/1</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/ComponentDefinition_dvk_backbone_core/1</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
     <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/B0032/1</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/B0015/1</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>https://charmme.synbiohub.org/user/Gonza10V/CIDARMoCloKit/ComponentDefinition_dvk_backbone_core/1</t>
   </si>
   <si>
     <t>B1</t>

</xml_diff>